<commit_message>
oper research assignment final (?)
</commit_message>
<xml_diff>
--- a/semester A/Oper. Research/Assignment.xlsx
+++ b/semester A/Oper. Research/Assignment.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppapa\OneDrive\Υπολογιστής\MSC\semester A\Oper. Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A5E657-ADC4-40E9-BFFE-3AF3C7BC0656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C07B8B-5994-48B6-91C8-79C11F9296E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Answer Report" sheetId="3" r:id="rId1"/>
+    <sheet name="Answer Report" sheetId="4" r:id="rId1"/>
     <sheet name="Solver" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -30,8 +30,8 @@
     <definedName name="solver_lhs13" localSheetId="1" hidden="1">Solver!$G$9</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Solver!$G$10:$G$13</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Solver!$G$14</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Solver!$G$4:$G$9</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Solver!#REF!</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Solver!$G$16:$G$20</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Solver!$G$4:$G$9</definedName>
     <definedName name="solver_lhs6" localSheetId="1" hidden="1">Solver!$G$14</definedName>
     <definedName name="solver_lhs7" localSheetId="1" hidden="1">Solver!$G$4</definedName>
     <definedName name="solver_lhs8" localSheetId="1" hidden="1">Solver!$G$5</definedName>
@@ -42,7 +42,7 @@
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Solver!$G$2</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
@@ -67,8 +67,8 @@
     <definedName name="solver_rhs13" localSheetId="1" hidden="1">Solver!$I$9</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Solver!$I$10:$I$13</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">Solver!$I$14</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Solver!$I$4:$I$9</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Solver!#REF!</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Solver!$I$16:$I$20</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Solver!$I$4:$I$9</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">Solver!$I$15</definedName>
     <definedName name="solver_rhs7" localSheetId="1" hidden="1">Solver!$I$4</definedName>
     <definedName name="solver_rhs8" localSheetId="1" hidden="1">Solver!$I$5</definedName>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>&lt;=</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Microsoft Excel 16.0 Answer Report</t>
   </si>
   <si>
-    <t>Worksheet: [Assignment.xlsx]Sheet1</t>
-  </si>
-  <si>
     <t>Result: Solver found a solution.  All Constraints and optimality conditions are satisfied.</t>
   </si>
   <si>
@@ -272,20 +269,29 @@
     <t>$G$9&lt;=$I$9</t>
   </si>
   <si>
-    <t>Report Created: 12/25/2024 4:39:47 PM</t>
-  </si>
-  <si>
-    <t>Solution Time: 0.047 Seconds.</t>
-  </si>
-  <si>
     <t>$A$2:$F$2=Integer</t>
+  </si>
+  <si>
+    <t>Worksheet: [Assignment.xlsx]Solver</t>
+  </si>
+  <si>
+    <t>Report Created: 1/2/2025 2:14:10 PM</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.031 Seconds.</t>
+  </si>
+  <si>
+    <t>Περιττοι περιορισμοί για μελέτη</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Περιθώριο μείωσης </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +316,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -362,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -372,6 +391,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,138 +674,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D77024E-BB87-4FC9-9981-B718DCBF1E8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACACB47-10BD-4FE8-9288-EF4D55100581}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="5">
-        <v>478652600</v>
+        <v>486923000</v>
       </c>
       <c r="E16" s="5">
-        <v>478652600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>486923000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="6">
@@ -792,12 +815,12 @@
         <v>3500</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="6">
@@ -807,12 +830,12 @@
         <v>4000</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="6">
@@ -822,12 +845,12 @@
         <v>2000</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="6">
@@ -837,12 +860,12 @@
         <v>4000</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="6">
@@ -852,12 +875,12 @@
         <v>6600</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5">
@@ -867,235 +890,235 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="6">
         <v>7500</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="G31" s="6">
         <v>3700</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="6">
         <v>9500</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="6">
         <v>800</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="6">
         <v>13500</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="6">
         <v>20100</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="6">
         <v>3200</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="6">
         <v>20100</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="6">
         <v>3500</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="6">
         <v>4000</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="6">
         <v>2000</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G38" s="4">
         <v>2500</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="6">
         <v>4000</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="6">
         <v>6600</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G40" s="4">
         <v>3000</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="6">
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G41" s="4">
         <v>7200</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1110,39 +1133,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>24544</v>
+        <v>25044</v>
       </c>
       <c r="B1">
-        <v>24822</v>
+        <v>25722</v>
       </c>
       <c r="C1">
-        <v>25186</v>
+        <v>25886</v>
       </c>
       <c r="D1">
-        <v>25186</v>
+        <v>25543</v>
       </c>
       <c r="E1">
-        <v>24686</v>
+        <v>24700</v>
       </c>
       <c r="F1">
         <v>26364</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3500</v>
       </c>
@@ -1163,10 +1187,10 @@
       </c>
       <c r="G2">
         <f>SUMPRODUCT(A1:F1,$A$2:$F$2)-20583000</f>
-        <v>478652600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>486923000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1181,12 +1205,12 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G14" si="0">SUMPRODUCT(A5:F5,$A$2:$F$2)</f>
+        <f t="shared" ref="G5:G20" si="0">SUMPRODUCT(A5:F5,$A$2:$F$2)</f>
         <v>4000</v>
       </c>
       <c r="H5" t="s">
@@ -1196,7 +1220,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -1211,7 +1235,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>1</v>
       </c>
@@ -1226,7 +1250,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>1</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>1</v>
       </c>
@@ -1256,7 +1280,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1274,7 +1298,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1295,7 +1319,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1319,7 +1343,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1346,7 +1370,7 @@
         <v>16900</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1376,7 +1400,146 @@
         <v>20100</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="J15" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>4500</v>
+      </c>
+      <c r="J16">
+        <f>I16-G16</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>8300</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J20" si="1">I17-G17</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>9500</v>
+      </c>
+      <c r="H18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>13300</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>13500</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>18100</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>20100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>21500</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>